<commit_message>
images to the wines and spirits
</commit_message>
<xml_diff>
--- a/spirits.xlsx
+++ b/spirits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProiectProfuDeVin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70902A53-D2CF-4421-A307-675B1EEE6A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19D2F5D-C26D-4AC4-A9C1-27DA971EC076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Type</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>AlcLvl</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>spirits/image1.png</t>
   </si>
 </sst>
 </file>
@@ -199,15 +205,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F33" totalsRowShown="0">
-  <autoFilter ref="A1:F33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G33" totalsRowShown="0">
+  <autoFilter ref="A1:G33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Style"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="AlcLvl"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Price"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Qty"/>
+    <tableColumn id="7" xr3:uid="{B8FF7C6F-C7A6-49CB-B0BB-BD295F71F04F}" name="image"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -510,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,9 +530,10 @@
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,8 +552,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -561,8 +572,11 @@
       <c r="F2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -579,7 +593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -596,7 +610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -613,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -633,7 +647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -650,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -667,7 +681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -687,7 +701,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -704,7 +718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -721,7 +735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -741,7 +755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -761,7 +775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -781,7 +795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -798,7 +812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>

</xml_diff>